<commit_message>
start to model lot sizing rules
</commit_message>
<xml_diff>
--- a/Instances/01_Lumpy_b2_fe25_en_rk50_ll0_l20.xlsx
+++ b/Instances/01_Lumpy_b2_fe25_en_rk50_ll0_l20.xlsx
@@ -911,7 +911,7 @@
         <v>1</v>
       </c>
       <c r="C4" t="n">
-        <v>2122</v>
+        <v>837</v>
       </c>
       <c r="D4" t="n">
         <v>0.0048</v>
@@ -940,7 +940,7 @@
         <v>1</v>
       </c>
       <c r="C5" t="n">
-        <v>2122</v>
+        <v>837</v>
       </c>
       <c r="D5" t="n">
         <v>0.002</v>
@@ -969,7 +969,7 @@
         <v>1</v>
       </c>
       <c r="C6" t="n">
-        <v>2122</v>
+        <v>837</v>
       </c>
       <c r="D6" t="n">
         <v>0.0036</v>
@@ -998,7 +998,7 @@
         <v>1</v>
       </c>
       <c r="C7" t="n">
-        <v>2565</v>
+        <v>1013</v>
       </c>
       <c r="D7" t="n">
         <v>0.026</v>
@@ -1027,7 +1027,7 @@
         <v>1</v>
       </c>
       <c r="C8" t="n">
-        <v>465</v>
+        <v>181</v>
       </c>
       <c r="D8" t="n">
         <v>0.0508</v>
@@ -1056,7 +1056,7 @@
         <v>1</v>
       </c>
       <c r="C9" t="n">
-        <v>769</v>
+        <v>301</v>
       </c>
       <c r="D9" t="n">
         <v>0.0248</v>

</xml_diff>

<commit_message>
implement first version of lot sizing rules
</commit_message>
<xml_diff>
--- a/Instances/01_Lumpy_b2_fe25_en_rk50_ll0_l20.xlsx
+++ b/Instances/01_Lumpy_b2_fe25_en_rk50_ll0_l20.xlsx
@@ -480,7 +480,7 @@
         <v>3</v>
       </c>
       <c r="B4" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="5" spans="1:2">
@@ -911,7 +911,7 @@
         <v>1</v>
       </c>
       <c r="C4" t="n">
-        <v>837</v>
+        <v>1673</v>
       </c>
       <c r="D4" t="n">
         <v>0.0048</v>
@@ -940,7 +940,7 @@
         <v>1</v>
       </c>
       <c r="C5" t="n">
-        <v>837</v>
+        <v>1673</v>
       </c>
       <c r="D5" t="n">
         <v>0.002</v>
@@ -969,7 +969,7 @@
         <v>1</v>
       </c>
       <c r="C6" t="n">
-        <v>837</v>
+        <v>1673</v>
       </c>
       <c r="D6" t="n">
         <v>0.0036</v>
@@ -1088,7 +1088,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I4"/>
+  <dimension ref="A1:I5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1206,6 +1206,35 @@
         <v>45</v>
       </c>
       <c r="I4" t="n">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9">
+      <c r="A5" s="1" t="n">
+        <v>3</v>
+      </c>
+      <c r="B5" t="n">
+        <v>0</v>
+      </c>
+      <c r="C5" t="n">
+        <v>0</v>
+      </c>
+      <c r="D5" t="n">
+        <v>0</v>
+      </c>
+      <c r="E5" t="n">
+        <v>0</v>
+      </c>
+      <c r="F5" t="n">
+        <v>0</v>
+      </c>
+      <c r="G5" t="n">
+        <v>253</v>
+      </c>
+      <c r="H5" t="n">
+        <v>45</v>
+      </c>
+      <c r="I5" t="n">
         <v>75</v>
       </c>
     </row>
@@ -1220,7 +1249,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I4"/>
+  <dimension ref="A1:I5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1338,6 +1367,35 @@
         <v>1</v>
       </c>
       <c r="I4" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9">
+      <c r="A5" s="1" t="n">
+        <v>3</v>
+      </c>
+      <c r="B5" t="n">
+        <v>0</v>
+      </c>
+      <c r="C5" t="n">
+        <v>0</v>
+      </c>
+      <c r="D5" t="n">
+        <v>0</v>
+      </c>
+      <c r="E5" t="n">
+        <v>0</v>
+      </c>
+      <c r="F5" t="n">
+        <v>0</v>
+      </c>
+      <c r="G5" t="n">
+        <v>36.62</v>
+      </c>
+      <c r="H5" t="n">
+        <v>1</v>
+      </c>
+      <c r="I5" t="n">
         <v>2</v>
       </c>
     </row>

</xml_diff>